<commit_message>
ver 1 with exe
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfredo\OneDrive\Desktop\advfinsa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfredo\OneDrive\Documents\GitHub\Advfinsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E700B6A2-0412-4B64-AF36-690B475E864A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F80348E-548A-4B4F-BC16-431BC7683A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{440B3108-3C37-40D6-9B34-D0714F6E856E}"/>
+    <workbookView xWindow="7800" yWindow="1020" windowWidth="10380" windowHeight="11712" xr2:uid="{440B3108-3C37-40D6-9B34-D0714F6E856E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,60 +36,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
     <t>tipo_persona</t>
   </si>
   <si>
-    <t>interpol</t>
-  </si>
-  <si>
-    <t>0925647851</t>
-  </si>
-  <si>
-    <t>Alfredo Gustavo Barandearan Gutierrez</t>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Nombres</t>
+  </si>
+  <si>
+    <t>Apellidos</t>
+  </si>
+  <si>
+    <t>0990071969001</t>
+  </si>
+  <si>
+    <t>EMPAGRAM</t>
+  </si>
+  <si>
+    <t>Juridica</t>
+  </si>
+  <si>
+    <t>0908894934</t>
+  </si>
+  <si>
+    <t>Alfredo Javier</t>
+  </si>
+  <si>
+    <t>Barandearan Oyague</t>
   </si>
   <si>
     <t>Natural</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Alfredo Javier Barandearan Oyagure</t>
-  </si>
-  <si>
-    <t>0908894934</t>
-  </si>
-  <si>
     <t>0914788245</t>
   </si>
   <si>
-    <t>Melania Sissi Gutierrez Gavilanes</t>
-  </si>
-  <si>
-    <t>0990071969001</t>
-  </si>
-  <si>
-    <t>EMPAGRAM</t>
-  </si>
-  <si>
-    <t>Juridica</t>
-  </si>
-  <si>
-    <t>Ariana Cristina Barandearan Gutierrez</t>
+    <t>Melania Sissi</t>
+  </si>
+  <si>
+    <t>Gutierrez Gavilanes</t>
   </si>
   <si>
     <t>0929029395</t>
+  </si>
+  <si>
+    <t>Ariana Cristina</t>
+  </si>
+  <si>
+    <t>Barandearan Gutierrez</t>
+  </si>
+  <si>
+    <t>1309022935</t>
+  </si>
+  <si>
+    <t>Jose Adolfo</t>
+  </si>
+  <si>
+    <t>Macias Villamar</t>
+  </si>
+  <si>
+    <t>1391791119001</t>
+  </si>
+  <si>
+    <t>Las Olas SA</t>
+  </si>
+  <si>
+    <t>0908890452</t>
+  </si>
+  <si>
+    <t>Roberto David</t>
+  </si>
+  <si>
+    <t>1709705675</t>
+  </si>
+  <si>
+    <t>Mary Paz</t>
+  </si>
+  <si>
+    <t>Herrera Oramas</t>
   </si>
 </sst>
 </file>
@@ -478,15 +508,15 @@
   <dimension ref="A2:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -494,64 +524,61 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>37598</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>24882</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3">
-        <v>24882</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>26669</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3">
-        <v>26669</v>
-      </c>
-      <c r="D5" t="s">
         <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>36526</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -559,53 +586,85 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3">
-        <v>36526</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3">
+        <v>38789</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3">
-        <v>38789</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3">
+        <v>29128</v>
       </c>
       <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3">
+        <v>36526</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="C8" s="3"/>
-    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
+        <v>28432</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="C11" s="3"/>
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="3">
+        <v>25441</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>

</xml_diff>